<commit_message>
Fix IE name issue, improve code, tweak test files
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/path_error.xlsx
+++ b/tests/integration_test_files/path_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBAE4BD-6ECD-3C49-AF45-13E8D4C7A740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E33EB7-F265-9B46-B20E-FC9908893F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51940" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="9" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="13060" yWindow="500" windowWidth="48440" windowHeight="27240" firstSheet="1" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="827">
   <si>
     <t>Screening</t>
   </si>
@@ -2560,6 +2560,9 @@
   </si>
   <si>
     <t>Secondary Objective</t>
+  </si>
+  <si>
+    <t>Age Criteria 2</t>
   </si>
 </sst>
 </file>
@@ -2801,13 +2804,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5362,7 +5365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7983,120 +7986,120 @@
       <c r="A1" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>815</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="51" t="s">
         <v>681</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="51" t="s">
         <v>712</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8188,16 +8191,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8209,8 +8212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8332,7 +8335,7 @@
         <v>813</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>584</v>
+        <v>826</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>585</v>
@@ -11840,15 +11843,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12049,6 +12043,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12061,14 +12064,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12083,6 +12078,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Test results and source file tweaks
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/path_error.xlsx
+++ b/tests/integration_test_files/path_error.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E33EB7-F265-9B46-B20E-FC9908893F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8812A2-F780-6341-91B9-610E03FCA903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="500" windowWidth="48440" windowHeight="27240" firstSheet="1" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="13060" yWindow="500" windowWidth="48440" windowHeight="27240" firstSheet="1" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="827">
   <si>
     <t>Screening</t>
   </si>
@@ -2804,13 +2804,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3365,7 +3365,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3576,9 +3576,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
         <v>168</v>
       </c>
@@ -3792,7 +3790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A98DD9-8159-D74D-B42C-CCC2F4D10811}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7986,120 +7984,120 @@
       <c r="A1" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>815</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>681</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>712</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8191,16 +8189,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8212,7 +8210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -8564,7 +8562,7 @@
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C25"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10441,9 +10439,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A36" s="5"/>
       <c r="B36" s="3" t="s">
         <v>168</v>
       </c>
@@ -11843,6 +11839,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12043,15 +12048,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12064,6 +12060,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12078,14 +12082,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>